<commit_message>
Fixed some header values
</commit_message>
<xml_diff>
--- a/tests/importer/metadata_spleen_new_protocols.xlsx
+++ b/tests/importer/metadata_spleen_new_protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaclan/dev/hca/latest/ingest-client/tests/importer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B4D45230-0F73-A644-875D-C15F40AC7C00}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BD4A018A-3414-2E43-9483-078DCCCA8047}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="680" windowWidth="25660" windowHeight="15660" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19460" yWindow="1840" windowWidth="28340" windowHeight="20960" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="493">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -993,9 +993,6 @@
   </si>
   <si>
     <t>library_preparation_protocol.protocol_type.ontology</t>
-  </si>
-  <si>
-    <t>sequencing_protocol.process_core.process_id</t>
   </si>
   <si>
     <t>sequencing_protocol.process_core.process_name</t>
@@ -2112,22 +2109,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>386</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -2139,7 +2136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2159,34 +2156,34 @@
     <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="270" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="120" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>51</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
@@ -2195,34 +2192,34 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>205</v>
@@ -2233,45 +2230,45 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H4" t="s">
         <v>209</v>
       </c>
       <c r="I4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K4" t="s">
         <v>205</v>
@@ -2287,89 +2284,89 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>480</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="D6" t="s">
         <v>481</v>
-      </c>
-      <c r="D6" t="s">
-        <v>482</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="D7" t="s">
         <v>484</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="D7" t="s">
-        <v>485</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L7" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="D8" t="s">
         <v>486</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="D8" t="s">
-        <v>487</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L8" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -2381,83 +2378,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -2593,240 +2592,240 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>389</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>394</v>
-      </c>
       <c r="H6" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>395</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>396</v>
-      </c>
       <c r="C7" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>394</v>
-      </c>
       <c r="H7" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>398</v>
-      </c>
       <c r="C8" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>390</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>394</v>
-      </c>
       <c r="H8" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>399</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>400</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>394</v>
-      </c>
       <c r="H9" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>400</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>401</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>402</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>405</v>
-      </c>
       <c r="G10" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>406</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>407</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>405</v>
-      </c>
       <c r="G11" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>408</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>409</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>411</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>412</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="B14" t="s">
         <v>413</v>
       </c>
-      <c r="B14" t="s">
-        <v>414</v>
-      </c>
       <c r="D14" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F14" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>393</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>394</v>
-      </c>
       <c r="H14" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>416</v>
-      </c>
       <c r="D15" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -2839,7 +2838,7 @@
   <dimension ref="A1:AO6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3227,77 +3226,77 @@
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>418</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>419</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
       </c>
       <c r="H6" s="10"/>
       <c r="M6" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="N6" t="s">
         <v>420</v>
       </c>
-      <c r="N6" t="s">
+      <c r="R6" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="U6" s="7" t="s">
         <v>422</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="X6" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="X6" s="7" t="s">
+      <c r="Y6" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="Y6" s="7" t="s">
+      <c r="Z6" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="Z6" s="7" t="s">
+      <c r="AA6" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="AA6" s="7" t="s">
+      <c r="AB6" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="AB6" s="7" t="s">
+      <c r="AC6" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="AC6" s="7" t="s">
+      <c r="AD6" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="AD6" s="7" t="s">
+      <c r="AE6" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="AE6" s="7" t="s">
+      <c r="AG6" s="7" t="s">
         <v>431</v>
       </c>
-      <c r="AG6" s="7" t="s">
+      <c r="AH6" t="s">
         <v>432</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="AI6" s="7" t="s">
+      <c r="AJ6" t="s">
         <v>434</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>435</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" s="11" t="s">
         <v>436</v>
       </c>
-      <c r="AL6" s="11" t="s">
+      <c r="AM6" t="s">
         <v>437</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>438</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>439</v>
       </c>
       <c r="AO6" s="12"/>
     </row>
@@ -3310,42 +3309,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
-    <col min="11" max="14" width="0" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="34.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="17.6640625" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" customWidth="1"/>
-    <col min="21" max="21" width="23.6640625" customWidth="1"/>
-    <col min="22" max="22" width="17.6640625" customWidth="1"/>
-    <col min="23" max="23" width="20.6640625" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" customWidth="1"/>
-    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="14.6640625" customWidth="1"/>
-    <col min="28" max="28" width="18.6640625" customWidth="1"/>
-    <col min="29" max="29" width="31.6640625" customWidth="1"/>
-    <col min="30" max="30" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="54" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="47.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="53.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="51" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="55.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="360" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -3619,44 +3621,44 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>441</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>442</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>424</v>
-      </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="7" t="s">
         <v>444</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>445</v>
       </c>
       <c r="N6" s="11"/>
       <c r="R6" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="S6" t="s">
         <v>446</v>
-      </c>
-      <c r="S6" t="s">
-        <v>447</v>
       </c>
       <c r="T6" s="7">
         <v>7200</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="W6" s="7">
         <v>19800</v>
@@ -3671,43 +3673,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AB6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
-    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" customWidth="1"/>
-    <col min="19" max="19" width="25.6640625" customWidth="1"/>
-    <col min="20" max="20" width="26.6640625" customWidth="1"/>
-    <col min="21" max="21" width="14.6640625" customWidth="1"/>
-    <col min="22" max="22" width="0" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" customWidth="1"/>
-    <col min="24" max="24" width="26.6640625" customWidth="1"/>
-    <col min="25" max="25" width="47.6640625" customWidth="1"/>
-    <col min="26" max="26" width="45.6640625" customWidth="1"/>
-    <col min="27" max="27" width="31.6640625" customWidth="1"/>
-    <col min="28" max="28" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="41.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="51" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="360" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="105" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -3976,34 +3976,34 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>449</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>450</v>
       </c>
       <c r="D6" s="7">
         <v>9606</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I6" t="s">
+        <v>450</v>
+      </c>
+      <c r="J6" t="s">
         <v>451</v>
       </c>
-      <c r="J6" t="s">
-        <v>452</v>
-      </c>
       <c r="V6" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="X6" s="13">
         <v>39300000</v>
       </c>
       <c r="Y6" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="Z6" t="s">
         <v>453</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -4124,25 +4124,25 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B6" t="s">
+        <v>454</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" t="s">
         <v>456</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>457</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>458</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" s="14" t="s">
         <v>459</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -4278,16 +4278,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>461</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="G6" t="s">
         <v>462</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>463</v>
-      </c>
-      <c r="H6" t="s">
-        <v>464</v>
       </c>
       <c r="L6" s="7"/>
     </row>
@@ -4627,13 +4627,13 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B6" t="s">
         <v>465</v>
       </c>
-      <c r="B6" t="s">
+      <c r="G6" t="s">
         <v>466</v>
-      </c>
-      <c r="G6" t="s">
-        <v>467</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -4642,22 +4642,22 @@
         <v>16</v>
       </c>
       <c r="K6" s="15" t="s">
+        <v>467</v>
+      </c>
+      <c r="L6" s="15" t="s">
         <v>468</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="M6" t="s">
         <v>469</v>
       </c>
-      <c r="M6" t="s">
+      <c r="X6" t="s">
         <v>470</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="Z6" s="9" t="s">
-        <v>472</v>
-      </c>
       <c r="AG6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AH6">
         <v>16</v>
@@ -4666,7 +4666,7 @@
         <v>10</v>
       </c>
       <c r="AL6" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -4678,8 +4678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4714,10 +4714,10 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>125</v>
@@ -4725,92 +4725,92 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>493</v>
-      </c>
       <c r="G2" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>332</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B4" t="s">
         <v>321</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>322</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>323</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>324</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>325</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>326</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>327</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>328</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>329</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>330</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>331</v>
       </c>
-      <c r="L4" t="s">
-        <v>332</v>
-      </c>
       <c r="M4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N4" t="s">
+        <v>336</v>
+      </c>
+      <c r="O4" t="s">
         <v>337</v>
-      </c>
-      <c r="O4" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -4820,34 +4820,34 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>473</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="C6" s="16" t="s">
         <v>474</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="G6" t="s">
         <v>475</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>476</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>477</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" s="6" t="s">
         <v>478</v>
       </c>
-      <c r="K6" s="6" t="s">
-        <v>479</v>
-      </c>
       <c r="M6" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="N6" t="s">
+        <v>458</v>
+      </c>
+      <c r="O6" s="14" t="s">
         <v>459</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed process column in Files tab
</commit_message>
<xml_diff>
--- a/tests/importer/metadata_spleen_new_protocols.xlsx
+++ b/tests/importer/metadata_spleen_new_protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaclan/dev/hca/latest/ingest-client/tests/importer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BD4A018A-3414-2E43-9483-078DCCCA8047}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{53A5D060-2ADD-4841-9C9A-EB3AAFD56DBA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19460" yWindow="1840" windowWidth="28340" windowHeight="20960" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8140" yWindow="960" windowWidth="28340" windowHeight="20960" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="492">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -1511,9 +1511,6 @@
   </si>
   <si>
     <t>read2</t>
-  </si>
-  <si>
-    <t>p1</t>
   </si>
   <si>
     <t>sequencing_protocol.protocol_core.process_name</t>
@@ -2136,8 +2133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2186,9 +2183,7 @@
         <v>363</v>
       </c>
       <c r="K1" s="1"/>
-      <c r="L1" s="1" t="s">
-        <v>206</v>
-      </c>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2224,9 +2219,7 @@
       <c r="K2" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>207</v>
-      </c>
+      <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
@@ -2273,9 +2266,6 @@
       <c r="K4" t="s">
         <v>205</v>
       </c>
-      <c r="L4" t="s">
-        <v>208</v>
-      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -2307,9 +2297,6 @@
       <c r="J6" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="L6" t="s">
-        <v>487</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -2336,9 +2323,6 @@
       <c r="J7" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="L7" t="s">
-        <v>487</v>
-      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
@@ -2364,9 +2348,6 @@
       </c>
       <c r="J8" s="7" t="s">
         <v>472</v>
-      </c>
-      <c r="L8" t="s">
-        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -2379,10 +2360,13 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="80.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4678,7 +4662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -4728,19 +4712,19 @@
         <v>365</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>489</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>490</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>491</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>492</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>326</v>

</xml_diff>

<commit_message>
Refactored linking and submission
</commit_message>
<xml_diff>
--- a/tests/importer/metadata_spleen_new_protocols.xlsx
+++ b/tests/importer/metadata_spleen_new_protocols.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaclan/dev/hca/latest/ingest-client/tests/importer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{53A5D060-2ADD-4841-9C9A-EB3AAFD56DBA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{65B017E6-6705-3842-8AC4-D5B4B67326A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8140" yWindow="960" windowWidth="28340" windowHeight="20960" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="493">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -1526,6 +1526,9 @@
   </si>
   <si>
     <t>sequencing_protocol.protocol_core.operator_identity</t>
+  </si>
+  <si>
+    <t>p1</t>
   </si>
 </sst>
 </file>
@@ -2150,7 +2153,6 @@
     <col min="9" max="9" width="45.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="120" x14ac:dyDescent="0.2">
@@ -2183,7 +2185,9 @@
         <v>363</v>
       </c>
       <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -2219,7 +2223,9 @@
       <c r="K2" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
@@ -2266,6 +2272,9 @@
       <c r="K4" t="s">
         <v>205</v>
       </c>
+      <c r="L4" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -2297,6 +2306,9 @@
       <c r="J6" s="7" t="s">
         <v>472</v>
       </c>
+      <c r="L6" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
@@ -2323,6 +2335,9 @@
       <c r="J7" s="7" t="s">
         <v>472</v>
       </c>
+      <c r="L7" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
@@ -2348,6 +2363,9 @@
       </c>
       <c r="J8" s="7" t="s">
         <v>472</v>
+      </c>
+      <c r="L8" t="s">
+        <v>492</v>
       </c>
     </row>
   </sheetData>

</xml_diff>